<commit_message>
added xgboost and adaboost to  cml1_scores.xlsx
</commit_message>
<xml_diff>
--- a/data/cml1_scores.xlsx
+++ b/data/cml1_scores.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\FHNW\Challenges\fhnw_ds_fs2021_medical_challenge\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70860CB4-26E1-4683-B614-B7EC67381410}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A2FCC3E-3874-437B-9CCE-8E53C36204D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7230" yWindow="2055" windowWidth="21600" windowHeight="11385" xr2:uid="{6A0542FE-781D-4799-8D04-B28DEDA5F814}"/>
+    <workbookView minimized="1" xWindow="6765" yWindow="4560" windowWidth="21600" windowHeight="11385" xr2:uid="{6A0542FE-781D-4799-8D04-B28DEDA5F814}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -38,6 +38,8 @@
   <authors>
     <author>tc={70128A9F-427C-4EEB-9BF5-6EABCBCA9157}</author>
     <author>tc={008B5A04-081B-49E9-8437-C3DF175E4FAE}</author>
+    <author>tc={82BC1B2E-3271-4757-8E18-63E41A7780BD}</author>
+    <author>tc={2E73208C-CFC8-4689-985D-FDF24DA49CD1}</author>
   </authors>
   <commentList>
     <comment ref="D10" authorId="0" shapeId="0" xr:uid="{70128A9F-427C-4EEB-9BF5-6EABCBCA9157}">
@@ -48,7 +50,23 @@
     Overfitted</t>
       </text>
     </comment>
-    <comment ref="M10" authorId="1" shapeId="0" xr:uid="{008B5A04-081B-49E9-8437-C3DF175E4FAE}">
+    <comment ref="O10" authorId="1" shapeId="0" xr:uid="{008B5A04-081B-49E9-8437-C3DF175E4FAE}">
+      <text>
+        <t>[Kommentarthread]
+Ihre Version von Excel gestattet Ihnen das Lesen dieses Kommentarthreads. Jegliche Bearbeitungen daran werden jedoch entfernt, wenn die Datei in einer neueren Version von Excel geöffnet wird. Weitere Informationen: https://go.microsoft.com/fwlink/?linkid=870924.
+Kommentar:
+    Overfitted</t>
+      </text>
+    </comment>
+    <comment ref="D29" authorId="2" shapeId="0" xr:uid="{82BC1B2E-3271-4757-8E18-63E41A7780BD}">
+      <text>
+        <t>[Kommentarthread]
+Ihre Version von Excel gestattet Ihnen das Lesen dieses Kommentarthreads. Jegliche Bearbeitungen daran werden jedoch entfernt, wenn die Datei in einer neueren Version von Excel geöffnet wird. Weitere Informationen: https://go.microsoft.com/fwlink/?linkid=870924.
+Kommentar:
+    Overfitted</t>
+      </text>
+    </comment>
+    <comment ref="O29" authorId="3" shapeId="0" xr:uid="{2E73208C-CFC8-4689-985D-FDF24DA49CD1}">
       <text>
         <t>[Kommentarthread]
 Ihre Version von Excel gestattet Ihnen das Lesen dieses Kommentarthreads. Jegliche Bearbeitungen daran werden jedoch entfernt, wenn die Datei in einer neueren Version von Excel geöffnet wird. Weitere Informationen: https://go.microsoft.com/fwlink/?linkid=870924.
@@ -61,7 +79,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="16">
   <si>
     <t>DecisionTree</t>
   </si>
@@ -104,6 +122,12 @@
   <si>
     <t xml:space="preserve">Zuletzt Bearbeitet: </t>
   </si>
+  <si>
+    <t>AdaBoost</t>
+  </si>
+  <si>
+    <t>XGBoost</t>
+  </si>
 </sst>
 </file>
 
@@ -129,7 +153,7 @@
       <sz val="9"/>
       <color indexed="81"/>
       <name val="Segoe UI"/>
-      <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="4">
@@ -152,7 +176,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -295,11 +319,50 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -319,6 +382,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -642,7 +721,13 @@
   <threadedComment ref="D10" dT="2021-05-16T10:39:42.22" personId="{2E33118D-8E94-4302-937A-52A8EF0E4118}" id="{70128A9F-427C-4EEB-9BF5-6EABCBCA9157}">
     <text>Overfitted</text>
   </threadedComment>
-  <threadedComment ref="M10" dT="2021-05-16T10:39:42.22" personId="{2E33118D-8E94-4302-937A-52A8EF0E4118}" id="{008B5A04-081B-49E9-8437-C3DF175E4FAE}">
+  <threadedComment ref="O10" dT="2021-05-16T10:39:42.22" personId="{2E33118D-8E94-4302-937A-52A8EF0E4118}" id="{008B5A04-081B-49E9-8437-C3DF175E4FAE}">
+    <text>Overfitted</text>
+  </threadedComment>
+  <threadedComment ref="D29" dT="2021-05-16T10:39:42.22" personId="{2E33118D-8E94-4302-937A-52A8EF0E4118}" id="{82BC1B2E-3271-4757-8E18-63E41A7780BD}">
+    <text>Overfitted</text>
+  </threadedComment>
+  <threadedComment ref="O29" dT="2021-05-16T10:39:42.22" personId="{2E33118D-8E94-4302-937A-52A8EF0E4118}" id="{2E73208C-CFC8-4689-985D-FDF24DA49CD1}">
     <text>Overfitted</text>
   </threadedComment>
 </ThreadedComments>
@@ -650,10 +735,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F7FD1A8-BA19-4FE0-84E1-74110D575CAB}">
-  <dimension ref="A1:Q17"/>
+  <dimension ref="A1:U32"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -662,27 +747,27 @@
     <col min="2" max="2" width="14.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14.5703125" customWidth="1"/>
     <col min="4" max="4" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="18" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="18" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B1" t="s">
         <v>11</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
+      <c r="M1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B3" s="4"/>
       <c r="C3" s="5" t="s">
         <v>8</v>
@@ -699,30 +784,42 @@
       <c r="G3" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="H3" s="6" t="s">
+      <c r="H3" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="I3" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="J3" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="K3" s="4"/>
-      <c r="L3" s="5" t="s">
+      <c r="M3" s="4"/>
+      <c r="N3" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="M3" s="5" t="s">
+      <c r="O3" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="N3" s="5" t="s">
+      <c r="P3" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="O3" s="5" t="s">
+      <c r="Q3" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="P3" s="5" t="s">
+      <c r="R3" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="Q3" s="6" t="s">
+      <c r="S3" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="T3" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="U3" s="6" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B4" s="7" t="s">
         <v>5</v>
       </c>
@@ -741,32 +838,44 @@
       <c r="G4" s="2">
         <v>0.21</v>
       </c>
-      <c r="H4" s="8">
+      <c r="H4" s="20">
+        <v>0.31</v>
+      </c>
+      <c r="I4" s="20">
+        <v>0.22</v>
+      </c>
+      <c r="J4" s="8">
         <v>0.32</v>
       </c>
-      <c r="K4" s="7" t="s">
+      <c r="M4" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="L4" s="2">
+      <c r="N4" s="2">
         <v>0.25</v>
       </c>
-      <c r="M4" s="2">
+      <c r="O4" s="2">
         <v>0.24</v>
       </c>
-      <c r="N4" s="2">
+      <c r="P4" s="2">
         <v>0.28999999999999998</v>
       </c>
-      <c r="O4" s="2">
+      <c r="Q4" s="2">
         <v>0.26</v>
       </c>
-      <c r="P4" s="2">
+      <c r="R4" s="2">
         <v>0.22</v>
       </c>
-      <c r="Q4" s="8">
+      <c r="S4" s="20">
+        <v>0.31</v>
+      </c>
+      <c r="T4" s="20">
+        <v>0.24</v>
+      </c>
+      <c r="U4" s="8">
         <v>0.32</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B5" s="7" t="s">
         <v>6</v>
       </c>
@@ -785,32 +894,44 @@
       <c r="G5" s="2">
         <v>0.27</v>
       </c>
-      <c r="H5" s="9">
+      <c r="H5" s="20">
+        <v>0.26</v>
+      </c>
+      <c r="I5" s="20">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="J5" s="9">
         <v>0.3</v>
       </c>
-      <c r="K5" s="7" t="s">
+      <c r="M5" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="L5" s="2">
+      <c r="N5" s="2">
         <v>0.32</v>
       </c>
-      <c r="M5" s="2">
+      <c r="O5" s="2">
         <v>0.26</v>
       </c>
-      <c r="N5" s="2">
+      <c r="P5" s="2">
         <v>0.27</v>
       </c>
-      <c r="O5" s="2">
+      <c r="Q5" s="2">
         <v>0.28000000000000003</v>
       </c>
-      <c r="P5" s="2">
+      <c r="R5" s="2">
         <v>0.28000000000000003</v>
       </c>
-      <c r="Q5" s="9">
+      <c r="S5" s="20">
+        <v>0.27</v>
+      </c>
+      <c r="T5" s="8">
+        <v>0.31</v>
+      </c>
+      <c r="U5" s="9">
         <v>0.3</v>
       </c>
     </row>
-    <row r="6" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B6" s="10" t="s">
         <v>7</v>
       </c>
@@ -829,47 +950,59 @@
       <c r="G6" s="11">
         <v>0.28000000000000003</v>
       </c>
-      <c r="H6" s="13">
+      <c r="H6" s="21">
+        <v>0.24</v>
+      </c>
+      <c r="I6" s="21">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="J6" s="13">
         <v>0.27</v>
       </c>
-      <c r="K6" s="10" t="s">
+      <c r="M6" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="L6" s="11">
+      <c r="N6" s="11">
         <v>0.26</v>
       </c>
-      <c r="M6" s="11">
+      <c r="O6" s="11">
         <v>0.25</v>
       </c>
-      <c r="N6" s="11">
+      <c r="P6" s="11">
         <v>0.31</v>
       </c>
-      <c r="O6" s="12">
+      <c r="Q6" s="12">
         <v>0.34</v>
       </c>
-      <c r="P6" s="11">
+      <c r="R6" s="11">
         <v>0.28000000000000003</v>
       </c>
-      <c r="Q6" s="13">
+      <c r="S6" s="21">
+        <v>0.27</v>
+      </c>
+      <c r="T6" s="21">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="U6" s="13">
         <v>0.3</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B8" t="s">
         <v>11</v>
       </c>
-      <c r="J8" s="1" t="s">
+      <c r="L8" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="K8" t="s">
+      <c r="M8" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B10" s="4"/>
       <c r="C10" s="5" t="s">
         <v>8</v>
@@ -886,30 +1019,42 @@
       <c r="G10" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="H10" s="6" t="s">
+      <c r="H10" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="I10" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="J10" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="K10" s="4"/>
-      <c r="L10" s="5" t="s">
+      <c r="M10" s="4"/>
+      <c r="N10" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="M10" s="5" t="s">
+      <c r="O10" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="N10" s="5" t="s">
+      <c r="P10" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="O10" s="5" t="s">
+      <c r="Q10" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="P10" s="5" t="s">
+      <c r="R10" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="Q10" s="6" t="s">
+      <c r="S10" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="T10" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="U10" s="6" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B11" s="7" t="s">
         <v>5</v>
       </c>
@@ -928,32 +1073,44 @@
       <c r="G11" s="3">
         <v>0.49</v>
       </c>
-      <c r="H11" s="8">
+      <c r="H11" s="22">
         <v>0.49</v>
       </c>
-      <c r="K11" s="7" t="s">
+      <c r="I11" s="22">
+        <v>0.51</v>
+      </c>
+      <c r="J11" s="8">
+        <v>0.49</v>
+      </c>
+      <c r="M11" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="L11" s="2">
+      <c r="N11" s="2">
         <v>0.56000000000000005</v>
       </c>
-      <c r="M11" s="2">
+      <c r="O11" s="2">
         <v>0.69</v>
       </c>
-      <c r="N11" s="2">
+      <c r="P11" s="2">
         <v>0.66</v>
       </c>
-      <c r="O11" s="3">
+      <c r="Q11" s="3">
         <v>0.69</v>
       </c>
-      <c r="P11" s="16">
+      <c r="R11" s="16">
         <v>0.55000000000000004</v>
       </c>
-      <c r="Q11" s="15">
+      <c r="S11" s="23">
+        <v>0.66</v>
+      </c>
+      <c r="T11" s="23">
+        <v>0.63</v>
+      </c>
+      <c r="U11" s="15">
         <v>0.57999999999999996</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B12" s="7" t="s">
         <v>6</v>
       </c>
@@ -972,32 +1129,44 @@
       <c r="G12" s="2">
         <v>0.52</v>
       </c>
-      <c r="H12" s="8">
+      <c r="H12" s="20">
+        <v>0.53</v>
+      </c>
+      <c r="I12" s="20">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="J12" s="8">
         <v>0.61</v>
       </c>
-      <c r="K12" s="7" t="s">
+      <c r="M12" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="L12" s="2">
+      <c r="N12" s="2">
         <v>0.6</v>
       </c>
-      <c r="M12" s="2">
+      <c r="O12" s="2">
         <v>0.73</v>
       </c>
-      <c r="N12" s="17">
+      <c r="P12" s="17">
         <v>0.68</v>
       </c>
-      <c r="O12" s="2">
+      <c r="Q12" s="2">
         <v>0.66</v>
       </c>
-      <c r="P12" s="2">
+      <c r="R12" s="2">
         <v>0.55000000000000004</v>
       </c>
-      <c r="Q12" s="8">
+      <c r="S12" s="20">
+        <v>0.66</v>
+      </c>
+      <c r="T12" s="20">
+        <v>0.64</v>
+      </c>
+      <c r="U12" s="8">
         <v>0.72</v>
       </c>
     </row>
-    <row r="13" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B13" s="10" t="s">
         <v>7</v>
       </c>
@@ -1016,38 +1185,404 @@
       <c r="G13" s="11">
         <v>0.52</v>
       </c>
-      <c r="H13" s="18">
+      <c r="H13" s="21">
+        <v>0.53</v>
+      </c>
+      <c r="I13" s="21">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="J13" s="18">
         <v>0.54</v>
       </c>
-      <c r="K13" s="10" t="s">
+      <c r="M13" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="L13" s="11">
+      <c r="N13" s="11">
         <v>0.6</v>
       </c>
-      <c r="M13" s="11">
+      <c r="O13" s="11">
         <v>0.64</v>
       </c>
-      <c r="N13" s="12">
+      <c r="P13" s="12">
         <v>0.64</v>
       </c>
-      <c r="O13" s="11">
+      <c r="Q13" s="11">
         <v>0.61</v>
       </c>
-      <c r="P13" s="11">
+      <c r="R13" s="11">
         <v>0.55000000000000004</v>
       </c>
-      <c r="Q13" s="13">
+      <c r="S13" s="21">
+        <v>0.62</v>
+      </c>
+      <c r="T13" s="21">
+        <v>0.63</v>
+      </c>
+      <c r="U13" s="13">
         <v>0.57999999999999996</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>13</v>
       </c>
       <c r="B17" s="14">
-        <v>44332</v>
-      </c>
+        <v>44347</v>
+      </c>
+    </row>
+    <row r="20" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B20" t="s">
+        <v>11</v>
+      </c>
+      <c r="L20" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="M20" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="21" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="22" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="B22" s="24"/>
+      <c r="C22" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="D22" s="25" t="s">
+        <v>0</v>
+      </c>
+      <c r="E22" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="F22" s="25" t="s">
+        <v>2</v>
+      </c>
+      <c r="G22" s="25" t="s">
+        <v>3</v>
+      </c>
+      <c r="H22" s="26" t="s">
+        <v>15</v>
+      </c>
+      <c r="I22" s="26" t="s">
+        <v>14</v>
+      </c>
+      <c r="J22" s="27" t="s">
+        <v>4</v>
+      </c>
+      <c r="K22" s="33"/>
+      <c r="L22" s="33"/>
+      <c r="M22" s="24"/>
+      <c r="N22" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="O22" s="25" t="s">
+        <v>0</v>
+      </c>
+      <c r="P22" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q22" s="25" t="s">
+        <v>2</v>
+      </c>
+      <c r="R22" s="25" t="s">
+        <v>3</v>
+      </c>
+      <c r="S22" s="26" t="s">
+        <v>15</v>
+      </c>
+      <c r="T22" s="26" t="s">
+        <v>14</v>
+      </c>
+      <c r="U22" s="27" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="B23" s="28" t="s">
+        <v>5</v>
+      </c>
+      <c r="C23" s="16"/>
+      <c r="D23" s="16"/>
+      <c r="E23" s="16"/>
+      <c r="F23" s="16"/>
+      <c r="G23" s="16"/>
+      <c r="H23" s="23"/>
+      <c r="I23" s="23"/>
+      <c r="J23" s="15"/>
+      <c r="K23" s="33"/>
+      <c r="L23" s="33"/>
+      <c r="M23" s="28" t="s">
+        <v>5</v>
+      </c>
+      <c r="N23" s="16"/>
+      <c r="O23" s="16"/>
+      <c r="P23" s="16"/>
+      <c r="Q23" s="16"/>
+      <c r="R23" s="16"/>
+      <c r="S23" s="23"/>
+      <c r="T23" s="23"/>
+      <c r="U23" s="15"/>
+    </row>
+    <row r="24" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="B24" s="28" t="s">
+        <v>6</v>
+      </c>
+      <c r="C24" s="16"/>
+      <c r="D24" s="16"/>
+      <c r="E24" s="16"/>
+      <c r="F24" s="16"/>
+      <c r="G24" s="16"/>
+      <c r="H24" s="23"/>
+      <c r="I24" s="23"/>
+      <c r="J24" s="15"/>
+      <c r="K24" s="33"/>
+      <c r="L24" s="33"/>
+      <c r="M24" s="28" t="s">
+        <v>6</v>
+      </c>
+      <c r="N24" s="16"/>
+      <c r="O24" s="16"/>
+      <c r="P24" s="16"/>
+      <c r="Q24" s="16"/>
+      <c r="R24" s="16"/>
+      <c r="S24" s="23"/>
+      <c r="T24" s="15"/>
+      <c r="U24" s="15"/>
+    </row>
+    <row r="25" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B25" s="29" t="s">
+        <v>7</v>
+      </c>
+      <c r="C25" s="30"/>
+      <c r="D25" s="30"/>
+      <c r="E25" s="30"/>
+      <c r="F25" s="30"/>
+      <c r="G25" s="30"/>
+      <c r="H25" s="31"/>
+      <c r="I25" s="31"/>
+      <c r="J25" s="32"/>
+      <c r="K25" s="33"/>
+      <c r="L25" s="33"/>
+      <c r="M25" s="29" t="s">
+        <v>7</v>
+      </c>
+      <c r="N25" s="30"/>
+      <c r="O25" s="30"/>
+      <c r="P25" s="30"/>
+      <c r="Q25" s="30"/>
+      <c r="R25" s="30"/>
+      <c r="S25" s="31"/>
+      <c r="T25" s="31"/>
+      <c r="U25" s="32"/>
+    </row>
+    <row r="26" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="B26" s="33"/>
+      <c r="C26" s="33"/>
+      <c r="D26" s="33"/>
+      <c r="E26" s="33"/>
+      <c r="F26" s="33"/>
+      <c r="G26" s="33"/>
+      <c r="H26" s="33"/>
+      <c r="I26" s="33"/>
+      <c r="J26" s="33"/>
+      <c r="K26" s="33"/>
+      <c r="L26" s="33"/>
+      <c r="M26" s="33"/>
+      <c r="N26" s="33"/>
+      <c r="O26" s="33"/>
+      <c r="P26" s="33"/>
+      <c r="Q26" s="33"/>
+      <c r="R26" s="33"/>
+      <c r="S26" s="33"/>
+      <c r="T26" s="33"/>
+      <c r="U26" s="33"/>
+    </row>
+    <row r="27" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B27" s="33" t="s">
+        <v>11</v>
+      </c>
+      <c r="C27" s="33"/>
+      <c r="D27" s="33"/>
+      <c r="E27" s="33"/>
+      <c r="F27" s="33"/>
+      <c r="G27" s="33"/>
+      <c r="H27" s="33"/>
+      <c r="I27" s="33"/>
+      <c r="J27" s="33"/>
+      <c r="K27" s="33"/>
+      <c r="L27" s="34" t="s">
+        <v>10</v>
+      </c>
+      <c r="M27" s="33" t="s">
+        <v>12</v>
+      </c>
+      <c r="N27" s="33"/>
+      <c r="O27" s="33"/>
+      <c r="P27" s="33"/>
+      <c r="Q27" s="33"/>
+      <c r="R27" s="33"/>
+      <c r="S27" s="33"/>
+      <c r="T27" s="33"/>
+      <c r="U27" s="33"/>
+    </row>
+    <row r="28" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B28" s="33"/>
+      <c r="C28" s="33"/>
+      <c r="D28" s="33"/>
+      <c r="E28" s="33"/>
+      <c r="F28" s="33"/>
+      <c r="G28" s="33"/>
+      <c r="H28" s="33"/>
+      <c r="I28" s="33"/>
+      <c r="J28" s="33"/>
+      <c r="K28" s="33"/>
+      <c r="L28" s="33"/>
+      <c r="M28" s="33"/>
+      <c r="N28" s="33"/>
+      <c r="O28" s="33"/>
+      <c r="P28" s="33"/>
+      <c r="Q28" s="33"/>
+      <c r="R28" s="33"/>
+      <c r="S28" s="33"/>
+      <c r="T28" s="33"/>
+      <c r="U28" s="33"/>
+    </row>
+    <row r="29" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="B29" s="24"/>
+      <c r="C29" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="D29" s="25" t="s">
+        <v>0</v>
+      </c>
+      <c r="E29" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="F29" s="25" t="s">
+        <v>2</v>
+      </c>
+      <c r="G29" s="25" t="s">
+        <v>3</v>
+      </c>
+      <c r="H29" s="26" t="s">
+        <v>15</v>
+      </c>
+      <c r="I29" s="26" t="s">
+        <v>14</v>
+      </c>
+      <c r="J29" s="27" t="s">
+        <v>4</v>
+      </c>
+      <c r="K29" s="33"/>
+      <c r="L29" s="33"/>
+      <c r="M29" s="24"/>
+      <c r="N29" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="O29" s="25" t="s">
+        <v>0</v>
+      </c>
+      <c r="P29" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q29" s="25" t="s">
+        <v>2</v>
+      </c>
+      <c r="R29" s="25" t="s">
+        <v>3</v>
+      </c>
+      <c r="S29" s="26" t="s">
+        <v>15</v>
+      </c>
+      <c r="T29" s="26" t="s">
+        <v>14</v>
+      </c>
+      <c r="U29" s="27" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="30" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="B30" s="28" t="s">
+        <v>5</v>
+      </c>
+      <c r="C30" s="16"/>
+      <c r="D30" s="16"/>
+      <c r="E30" s="16"/>
+      <c r="F30" s="16"/>
+      <c r="G30" s="16"/>
+      <c r="H30" s="23"/>
+      <c r="I30" s="23"/>
+      <c r="J30" s="15"/>
+      <c r="K30" s="33"/>
+      <c r="L30" s="33"/>
+      <c r="M30" s="28" t="s">
+        <v>5</v>
+      </c>
+      <c r="N30" s="16"/>
+      <c r="O30" s="16"/>
+      <c r="P30" s="16"/>
+      <c r="Q30" s="16"/>
+      <c r="R30" s="16"/>
+      <c r="S30" s="23"/>
+      <c r="T30" s="23"/>
+      <c r="U30" s="15"/>
+    </row>
+    <row r="31" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="B31" s="28" t="s">
+        <v>6</v>
+      </c>
+      <c r="C31" s="16"/>
+      <c r="D31" s="16"/>
+      <c r="E31" s="16"/>
+      <c r="F31" s="16"/>
+      <c r="G31" s="16"/>
+      <c r="H31" s="23"/>
+      <c r="I31" s="23"/>
+      <c r="J31" s="15"/>
+      <c r="K31" s="33"/>
+      <c r="L31" s="33"/>
+      <c r="M31" s="28" t="s">
+        <v>6</v>
+      </c>
+      <c r="N31" s="16"/>
+      <c r="O31" s="16"/>
+      <c r="P31" s="16"/>
+      <c r="Q31" s="16"/>
+      <c r="R31" s="16"/>
+      <c r="S31" s="23"/>
+      <c r="T31" s="23"/>
+      <c r="U31" s="15"/>
+    </row>
+    <row r="32" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B32" s="29" t="s">
+        <v>7</v>
+      </c>
+      <c r="C32" s="30"/>
+      <c r="D32" s="30"/>
+      <c r="E32" s="30"/>
+      <c r="F32" s="30"/>
+      <c r="G32" s="30"/>
+      <c r="H32" s="31"/>
+      <c r="I32" s="31"/>
+      <c r="J32" s="32"/>
+      <c r="K32" s="33"/>
+      <c r="L32" s="33"/>
+      <c r="M32" s="29" t="s">
+        <v>7</v>
+      </c>
+      <c r="N32" s="30"/>
+      <c r="O32" s="30"/>
+      <c r="P32" s="30"/>
+      <c r="Q32" s="30"/>
+      <c r="R32" s="30"/>
+      <c r="S32" s="31"/>
+      <c r="T32" s="31"/>
+      <c r="U32" s="32"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>